<commit_message>
lots of new files
</commit_message>
<xml_diff>
--- a/Application Number.xlsx
+++ b/Application Number.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Desktop\MaxBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC618E6-02F4-4FCD-86E2-0C7F2D13628C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370D6C79-F146-487A-BDEC-183A9601B45B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -456,7 +456,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>